<commit_message>
WBS primera entrega primeras actividades
</commit_message>
<xml_diff>
--- a/Avance.xlsx
+++ b/Avance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="270" yWindow="585" windowWidth="19815" windowHeight="7110"/>
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Hoja1!$B$2:$E$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Hoja1!$B$2:$E$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
@@ -20,13 +20,13 @@
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Hoja1"</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Hoja3"</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterate="1"/>
+  <calcPr calcId="124519"/>
   <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="121">
   <si>
     <t>Sebastian</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Modelo de proceso</t>
   </si>
   <si>
-    <t>Spiral, faltan actividades</t>
-  </si>
-  <si>
     <t>Faltan detalles</t>
   </si>
   <si>
@@ -362,12 +359,6 @@
   </si>
   <si>
     <t>Plan de evaluacion de nuevas herramientas y apps</t>
-  </si>
-  <si>
-    <t>9.3</t>
-  </si>
-  <si>
-    <t>Plan de integracion</t>
   </si>
   <si>
     <t>Porcentaje</t>
@@ -403,8 +394,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <b/>
       <sz val="11"/>
@@ -688,7 +679,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -723,7 +713,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -899,14 +888,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="58.7109375" customWidth="1"/>
@@ -916,7 +905,7 @@
     <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -932,7 +921,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -950,7 +939,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -965,7 +954,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="8">
-        <f>COUNTIF(E3:E101,3)</f>
+        <f>COUNTIF(E3:E100,3)</f>
         <v>6</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -973,7 +962,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
@@ -988,43 +977,43 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="10">
-        <f>COUNTIF(E3:E101,1)</f>
-        <v>10</v>
+        <f>COUNTIF(E3:E100,1)</f>
+        <v>9</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>20</v>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="E6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="11">
-        <f>COUNTIF(E3:E101,2)</f>
-        <v>10</v>
+        <f>COUNTIF(E3:E100,2)</f>
+        <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>2</v>
@@ -1034,87 +1023,89 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="14">
-        <f>COUNTIF(E3:E101,0)</f>
-        <v>16</v>
+        <f>COUNTIF(E3:E100,0)</f>
+        <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="15">
         <f>G5+G6+G4</f>
+        <v>28</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="16">
         <f>(G8/G11)</f>
-        <v>0.61904761904761907</v>
+        <v>0.68292682926829273</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>0</v>
+      </c>
       <c r="E10" s="7">
         <v>0</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="16">
         <f>(G5+G4)/G11</f>
-        <v>0.38095238095238093</v>
+        <v>0.36585365853658536</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
@@ -1124,20 +1115,20 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="18">
-        <f>COUNT(E3:E101)</f>
-        <v>42</v>
+        <f>COUNT(E3:E100)</f>
+        <v>41</v>
       </c>
       <c r="H11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>1</v>
@@ -1150,15 +1141,15 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
@@ -1168,12 +1159,12 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9">
       <c r="B14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="7">
@@ -1184,16 +1175,16 @@
         <v>0</v>
       </c>
       <c r="H14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>4</v>
@@ -1206,16 +1197,16 @@
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>4</v>
@@ -1228,16 +1219,16 @@
         <v>2</v>
       </c>
       <c r="H16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1250,48 +1241,48 @@
         <v>3</v>
       </c>
       <c r="H17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="17"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9">
       <c r="B19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="17"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>2</v>
@@ -1304,12 +1295,12 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>2</v>
@@ -1322,15 +1313,15 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>64</v>
       </c>
       <c r="E22" s="7">
         <v>2</v>
@@ -1340,12 +1331,12 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>2</v>
@@ -1358,12 +1349,12 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="7">
@@ -1374,12 +1365,12 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>2</v>
@@ -1392,12 +1383,12 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9">
       <c r="B26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="7">
@@ -1408,12 +1399,12 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>2</v>
@@ -1426,12 +1417,12 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="7">
@@ -1442,15 +1433,15 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" s="4">
         <v>7</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="E29" s="7">
         <v>2</v>
@@ -1460,12 +1451,12 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" s="4">
         <v>8</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="7">
@@ -1476,12 +1467,12 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="7">
@@ -1492,12 +1483,12 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="7">
@@ -1508,15 +1499,15 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="E33" s="7">
         <v>2</v>
@@ -1526,15 +1517,15 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="E34" s="7">
         <v>2</v>
@@ -1544,15 +1535,15 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="E35" s="7">
         <v>2</v>
@@ -1562,32 +1553,32 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="E36" s="7">
+        <v>2</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="E36" s="7">
-        <v>2</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9">
       <c r="B37" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>5</v>
@@ -1596,18 +1587,18 @@
         <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G37" s="21"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="7">
@@ -1618,12 +1609,12 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="D39" s="17"/>
       <c r="E39" s="7">
@@ -1634,12 +1625,12 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="7">
@@ -1650,12 +1641,12 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>1</v>
@@ -1668,14 +1659,16 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9">
       <c r="B42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="17"/>
+      <c r="D42" s="17" t="s">
+        <v>0</v>
+      </c>
       <c r="E42" s="7">
         <v>0</v>
       </c>
@@ -1684,14 +1677,16 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9">
       <c r="B43" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="17"/>
+      <c r="D43" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="E43" s="7">
         <v>0</v>
       </c>
@@ -1700,23 +1695,17 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="7">
-        <v>0</v>
-      </c>
+    <row r="44" spans="2:9">
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9">
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
@@ -1726,7 +1715,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9">
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="4"/>
@@ -1736,7 +1725,7 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9">
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="4"/>
@@ -1746,7 +1735,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9">
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="4"/>
@@ -1756,7 +1745,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9">
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="4"/>
@@ -1766,116 +1755,106 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <autoFilter ref="B2:E44"/>
+  <autoFilter ref="B2:E43"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" s="22"/>
       <c r="C4" s="23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
       <c r="B5" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C5" s="25">
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C6" s="25">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C7" s="25">
         <v>0.18</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3">
       <c r="B8" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C8" s="25">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3">
       <c r="B9" s="24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C9" s="25">
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" s="24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C10" s="25">
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3">
       <c r="B11" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C11" s="25">
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3">
       <c r="B12" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C12" s="25">
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3">
       <c r="B13" s="24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C13" s="25">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3">
       <c r="B14" s="26"/>
       <c r="C14" s="27"/>
     </row>
@@ -1886,14 +1865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="28"/>
     </row>
   </sheetData>

</xml_diff>